<commit_message>
mean and median push
</commit_message>
<xml_diff>
--- a/Tables/ClusterOversight.xlsx
+++ b/Tables/ClusterOversight.xlsx
@@ -456,13 +456,13 @@
         <v>0.120720697581247</v>
       </c>
       <c r="E2">
-        <v>0.9048669289296307</v>
+        <v>0.9048669289296306</v>
       </c>
       <c r="F2">
         <v>0.9922189188275892</v>
       </c>
       <c r="G2">
-        <v>0.4307694124029069</v>
+        <v>0.4307694124029075</v>
       </c>
       <c r="H2">
         <v>0.06260296235450927</v>
@@ -473,25 +473,25 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>0.9189908896166797</v>
+        <v>0.9623298439021065</v>
       </c>
       <c r="D3">
-        <v>0.6616385184807058</v>
+        <v>0.1028338431253394</v>
       </c>
       <c r="E3">
-        <v>0.9048669289296307</v>
+        <v>0.9048669289296306</v>
       </c>
       <c r="F3">
-        <v>0.6913029326157718</v>
+        <v>0.9975325979692565</v>
       </c>
       <c r="G3">
-        <v>0.8492948757379243</v>
+        <v>0.7975044194634193</v>
       </c>
       <c r="H3">
-        <v>0.6670279113914713</v>
+        <v>0.3326450380065146</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -499,25 +499,25 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>0.9241385728782294</v>
+        <v>0.9783479380831384</v>
       </c>
       <c r="D4">
-        <v>0.7330819931126085</v>
+        <v>0.2600292245963809</v>
       </c>
       <c r="E4">
         <v>0.9948012752887331</v>
       </c>
       <c r="F4">
-        <v>0.6913029326157718</v>
+        <v>0.9922189188275892</v>
       </c>
       <c r="G4">
-        <v>0.1654231913501785</v>
+        <v>0.1903475230646941</v>
       </c>
       <c r="H4">
-        <v>0.8990479535705495</v>
+        <v>0.2186635195045711</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -531,7 +531,7 @@
         <v>0.9777233743065304</v>
       </c>
       <c r="D5">
-        <v>0.1179100127470727</v>
+        <v>0.1179100127470729</v>
       </c>
       <c r="E5">
         <v>0.9975325979692565</v>
@@ -540,10 +540,10 @@
         <v>0.9922189188275892</v>
       </c>
       <c r="G5">
-        <v>0.9587888911066283</v>
+        <v>0.9587888911066282</v>
       </c>
       <c r="H5">
-        <v>0.1415496064188641</v>
+        <v>0.141549606418864</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -551,51 +551,51 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>0.9783479380831384</v>
+        <v>0.9657091117319888</v>
       </c>
       <c r="D6">
-        <v>0.2600292245963809</v>
+        <v>0.100073378760585</v>
       </c>
       <c r="E6">
         <v>0.9948012752887331</v>
       </c>
       <c r="F6">
-        <v>0.9922189188275892</v>
+        <v>0.9048669289296306</v>
       </c>
       <c r="G6">
-        <v>0.1903475230646939</v>
+        <v>0.3714655397054613</v>
       </c>
       <c r="H6">
-        <v>0.2186635195045715</v>
+        <v>0.3852252068075139</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
       <c r="C7">
-        <v>0.9097472141186467</v>
+        <v>0.9771805473804041</v>
       </c>
       <c r="D7">
-        <v>0.5355755997733357</v>
+        <v>0.2982061204769986</v>
       </c>
       <c r="E7">
+        <v>0.9948012752887331</v>
+      </c>
+      <c r="F7">
         <v>0.9975325979692565</v>
       </c>
-      <c r="F7">
-        <v>0.6913029326157718</v>
-      </c>
       <c r="G7">
-        <v>0.3779119866090961</v>
+        <v>0.9681175598233733</v>
       </c>
       <c r="H7">
-        <v>0.9347848457383898</v>
+        <v>0.224775862899768</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -603,25 +603,25 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C8">
-        <v>0.9657091117319888</v>
+        <v>0.9241385728782294</v>
       </c>
       <c r="D8">
-        <v>0.1000733787605839</v>
+        <v>0.7330819931126087</v>
       </c>
       <c r="E8">
         <v>0.9948012752887331</v>
       </c>
       <c r="F8">
-        <v>0.9048669289296307</v>
+        <v>0.6913029326157746</v>
       </c>
       <c r="G8">
-        <v>0.3714655397054611</v>
+        <v>0.165423191350179</v>
       </c>
       <c r="H8">
-        <v>0.3852252068075126</v>
+        <v>0.8990479535705498</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -635,16 +635,16 @@
         <v>0.8981858138266483</v>
       </c>
       <c r="D9">
-        <v>0.8417653326866765</v>
+        <v>0.8417653326866769</v>
       </c>
       <c r="E9">
         <v>0.9922189188275892</v>
       </c>
       <c r="F9">
-        <v>0.6913029326157718</v>
+        <v>0.6913029326157746</v>
       </c>
       <c r="G9">
-        <v>0.1817159148413598</v>
+        <v>0.1817159148413596</v>
       </c>
       <c r="H9">
         <v>0.8661209308406749</v>
@@ -652,28 +652,28 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C10">
-        <v>0.9771805473804041</v>
+        <v>0.9097472141186467</v>
       </c>
       <c r="D10">
-        <v>0.2982061204769981</v>
+        <v>0.5355755997733355</v>
       </c>
       <c r="E10">
-        <v>0.9948012752887331</v>
+        <v>0.9975325979692565</v>
       </c>
       <c r="F10">
-        <v>0.9975325979692565</v>
+        <v>0.6913029326157746</v>
       </c>
       <c r="G10">
-        <v>0.9681175598233734</v>
+        <v>0.3779119866090953</v>
       </c>
       <c r="H10">
-        <v>0.224775862899768</v>
+        <v>0.9347848457383896</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -681,25 +681,25 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C11">
-        <v>0.9623298439021065</v>
+        <v>0.9189908896166797</v>
       </c>
       <c r="D11">
-        <v>0.1028338431253394</v>
+        <v>0.6616385184807054</v>
       </c>
       <c r="E11">
-        <v>0.9048669289296307</v>
+        <v>0.9048669289296306</v>
       </c>
       <c r="F11">
-        <v>0.9975325979692565</v>
+        <v>0.6913029326157746</v>
       </c>
       <c r="G11">
-        <v>0.79750441946342</v>
+        <v>0.8492948757379242</v>
       </c>
       <c r="H11">
-        <v>0.3326450380065147</v>
+        <v>0.667027911391471</v>
       </c>
     </row>
   </sheetData>

</xml_diff>